<commit_message>
fix to double moon checklist
</commit_message>
<xml_diff>
--- a/double-moon-legend/checklist.xlsx
+++ b/double-moon-legend/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/double-moon-legend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{774B1DAF-B8DB-DA4F-A69A-E471C3AFC8E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628A246-C95C-A14E-9C78-AE75BFCCF101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{1E619BC3-096D-F442-B967-19D40EF54019}"/>
   </bookViews>
@@ -71,13 +71,13 @@
     <t>Double Moon Legend TRPG System Book</t>
   </si>
   <si>
-    <t>ダブルムーン伝説 TRPGスプリメントブック</t>
-  </si>
-  <si>
-    <t>ダブルムーン伝説システムブック</t>
-  </si>
-  <si>
     <t>Double Moon Legend Supplement Book</t>
+  </si>
+  <si>
+    <t>ダブルムーン伝説スプリメントブック</t>
+  </si>
+  <si>
+    <t>ダブルムーン伝説TRPGシステムブック</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,7 +477,7 @@
         <v>1991</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -500,7 +500,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>

</xml_diff>